<commit_message>
ching chong records changed to davis. Corrected formulae on IPO.
</commit_message>
<xml_diff>
--- a/CBLHJB02/CBLHJB02 IPO.xlsx
+++ b/CBLHJB02/CBLHJB02 IPO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\QAWI19\CBLHJB02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E334C2F8-F5B0-49A5-8B64-6B43B04FF3D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC10BD5C-08F0-4DC4-941C-8C565667AEFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14070" yWindow="5100" windowWidth="21600" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -139,9 +139,6 @@
     <t xml:space="preserve">BOB - DYLAN    </t>
   </si>
   <si>
-    <t xml:space="preserve">CHING CHONG    </t>
-  </si>
-  <si>
     <t xml:space="preserve">QUERVO         </t>
   </si>
   <si>
@@ -392,6 +389,9 @@
   </si>
   <si>
     <t>00250.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAVIS          </t>
   </si>
 </sst>
 </file>
@@ -556,6 +556,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -565,7 +566,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -848,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K83" sqref="K83:K92"/>
+    <sheetView tabSelected="1" topLeftCell="L64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R96" sqref="R96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,30 +875,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="36" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="38"/>
-      <c r="L1" s="36" t="s">
+      <c r="K1" s="39"/>
+      <c r="L1" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="39"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -911,28 +911,28 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>31</v>
       </c>
       <c r="H2" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="I2" s="33" t="s">
         <v>80</v>
-      </c>
-      <c r="I2" s="33" t="s">
-        <v>81</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>4</v>
@@ -961,19 +961,19 @@
         <v>33</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="24" t="s">
         <v>29</v>
       </c>
       <c r="D3" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>55</v>
-      </c>
       <c r="F3" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>13</v>
@@ -1004,7 +1004,7 @@
         <v>0</v>
       </c>
       <c r="O3" s="2" t="str">
-        <f t="shared" ref="O3:O12" si="4">CONCATENATE(E3,"/",F3,"/",RIGHT(D3,2))</f>
+        <f t="shared" ref="O3:O13" si="4">CONCATENATE(E3,"/",F3,"/",RIGHT(D3,2))</f>
         <v>12/11/19</v>
       </c>
       <c r="P3" s="2" t="str">
@@ -1022,22 +1022,22 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>118</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>13</v>
@@ -1046,7 +1046,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J4" s="13">
         <f t="shared" si="0"/>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="L4" s="1" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">CHING CHONG    </v>
+        <v xml:space="preserve">DAVIS          </v>
       </c>
       <c r="M4" s="2" t="str">
         <f t="shared" si="2"/>
@@ -1087,7 +1087,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>12</v>
@@ -1096,13 +1096,13 @@
         <v>19</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>13</v>
@@ -1111,7 +1111,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J5" s="13">
         <f t="shared" si="0"/>
@@ -1152,19 +1152,19 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>22</v>
@@ -1176,7 +1176,7 @@
         <v>3</v>
       </c>
       <c r="I6" s="34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J6" s="13">
         <f>TRUNC(C6+I6,2)</f>
@@ -1198,8 +1198,8 @@
         <f>VALUE(C6)</f>
         <v>10000</v>
       </c>
-      <c r="O6" s="7" t="str">
-        <f>CONCATENATE(E6,"/",F6,"/",RIGHT(D6,2))</f>
+      <c r="O6" s="2" t="str">
+        <f t="shared" si="4"/>
         <v>08/01/19</v>
       </c>
       <c r="P6" s="7" t="str">
@@ -1217,19 +1217,19 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>22</v>
@@ -1282,22 +1282,22 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="E8" s="15" t="s">
+      <c r="F8" s="16" t="s">
         <v>94</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>95</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>13</v>
@@ -1306,7 +1306,7 @@
         <v>2</v>
       </c>
       <c r="I8" s="34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J8" s="13">
         <f t="shared" si="0"/>
@@ -1328,7 +1328,10 @@
         <f t="shared" si="3"/>
         <v>50000</v>
       </c>
-      <c r="O8" s="2"/>
+      <c r="O8" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>03/23/80</v>
+      </c>
       <c r="P8" s="7" t="str">
         <f t="shared" si="7"/>
         <v>Ski Package</v>
@@ -1344,7 +1347,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>17</v>
@@ -1353,13 +1356,13 @@
         <v>19</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>13</v>
@@ -1409,22 +1412,22 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="24" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>13</v>
@@ -1474,22 +1477,22 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="24" t="s">
-        <v>49</v>
-      </c>
       <c r="D11" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>13</v>
@@ -1539,22 +1542,22 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" s="24" t="s">
         <v>29</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>13</v>
@@ -1563,7 +1566,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J12" s="13">
         <f t="shared" si="0"/>
@@ -1607,19 +1610,19 @@
         <v>32</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" s="24" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>13</v>
@@ -1651,7 +1654,7 @@
         <v>999999.99</v>
       </c>
       <c r="O13" s="2" t="str">
-        <f>CONCATENATE(E13,"/",F13,"/",RIGHT(D13,2))</f>
+        <f t="shared" si="4"/>
         <v>99/99/99</v>
       </c>
       <c r="P13" s="2" t="str">
@@ -1700,16 +1703,16 @@
       <c r="J15" s="13"/>
       <c r="K15" s="3"/>
       <c r="L15" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M15" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S15" s="1"/>
     </row>
@@ -1737,8 +1740,8 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="17">
-        <f>SUM(R3:R12)</f>
-        <v>2263000.0199999996</v>
+        <f>SUM(R3:R13)</f>
+        <v>3362999.9999999995</v>
       </c>
       <c r="S16" s="1"/>
     </row>
@@ -1767,19 +1770,19 @@
         <v>33</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" s="24" t="s">
         <v>29</v>
       </c>
       <c r="D18" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E18" s="14" t="s">
-        <v>55</v>
-      </c>
       <c r="F18" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>16</v>
@@ -1829,22 +1832,22 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>34</v>
+        <v>118</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>16</v>
@@ -1853,7 +1856,7 @@
         <v>1</v>
       </c>
       <c r="I19" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J19" s="13">
         <f t="shared" si="9"/>
@@ -1865,7 +1868,7 @@
       </c>
       <c r="L19" s="2" t="str">
         <f t="shared" si="10"/>
-        <v xml:space="preserve">CHING CHONG    </v>
+        <v xml:space="preserve">DAVIS          </v>
       </c>
       <c r="M19" s="2" t="str">
         <f t="shared" si="11"/>
@@ -1895,7 +1898,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>12</v>
@@ -1904,13 +1907,13 @@
         <v>19</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>16</v>
@@ -1919,7 +1922,7 @@
         <v>2</v>
       </c>
       <c r="I20" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J20" s="13">
         <f t="shared" si="9"/>
@@ -1961,19 +1964,19 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F21" s="16" t="s">
         <v>22</v>
@@ -2027,22 +2030,22 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C22" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="E22" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="16" t="s">
         <v>99</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>100</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>16</v>
@@ -2051,7 +2054,7 @@
         <v>2</v>
       </c>
       <c r="I22" s="34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J22" s="13">
         <f t="shared" si="9"/>
@@ -2093,7 +2096,7 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>17</v>
@@ -2102,13 +2105,13 @@
         <v>19</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>16</v>
@@ -2159,22 +2162,22 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C24" s="24" t="s">
         <v>29</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G24" s="7" t="s">
         <v>16</v>
@@ -2225,22 +2228,22 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="24" t="s">
-        <v>49</v>
-      </c>
       <c r="D25" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G25" s="7" t="s">
         <v>16</v>
@@ -2290,22 +2293,22 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C26" s="24" t="s">
         <v>29</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>16</v>
@@ -2314,7 +2317,7 @@
         <v>1</v>
       </c>
       <c r="I26" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J26" s="13">
         <f t="shared" si="9"/>
@@ -2355,22 +2358,22 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>16</v>
@@ -2379,7 +2382,7 @@
         <v>1</v>
       </c>
       <c r="I27" s="34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J27" s="13">
         <f t="shared" si="9"/>
@@ -2423,19 +2426,19 @@
         <v>32</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C28" s="24" t="s">
         <v>19</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>16</v>
@@ -2517,16 +2520,16 @@
       <c r="J30" s="13"/>
       <c r="K30" s="3"/>
       <c r="L30" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M30" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="M30" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
       <c r="R30" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
@@ -2553,8 +2556,8 @@
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
       <c r="R31" s="20">
-        <f>SUM(R18:R27)</f>
-        <v>2385000.0199999996</v>
+        <f>SUM(R18:R28)</f>
+        <v>3484999.9999999995</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
@@ -2581,19 +2584,19 @@
         <v>33</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C33" s="24" t="s">
         <v>29</v>
       </c>
       <c r="D33" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E33" s="14" t="s">
-        <v>55</v>
-      </c>
       <c r="F33" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>18</v>
@@ -2642,22 +2645,22 @@
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>34</v>
+        <v>118</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F34" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>18</v>
@@ -2666,7 +2669,7 @@
         <v>1</v>
       </c>
       <c r="I34" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J34" s="13">
         <f t="shared" si="18"/>
@@ -2678,7 +2681,7 @@
       </c>
       <c r="L34" s="2" t="str">
         <f t="shared" si="19"/>
-        <v xml:space="preserve">CHING CHONG    </v>
+        <v xml:space="preserve">DAVIS          </v>
       </c>
       <c r="M34" s="2" t="str">
         <f t="shared" si="20"/>
@@ -2707,22 +2710,22 @@
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C35" s="24" t="s">
+      <c r="D35" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E35" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="D35" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="E35" s="15" t="s">
-        <v>103</v>
-      </c>
       <c r="F35" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>18</v>
@@ -2731,7 +2734,7 @@
         <v>2</v>
       </c>
       <c r="I35" s="34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J35" s="13">
         <f t="shared" si="18"/>
@@ -2772,7 +2775,7 @@
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>12</v>
@@ -2781,13 +2784,13 @@
         <v>19</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F36" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G36" s="7" t="s">
         <v>18</v>
@@ -2796,7 +2799,7 @@
         <v>2</v>
       </c>
       <c r="I36" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J36" s="13">
         <f t="shared" si="18"/>
@@ -2837,19 +2840,19 @@
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F37" s="16" t="s">
         <v>22</v>
@@ -2902,7 +2905,7 @@
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>17</v>
@@ -2911,13 +2914,13 @@
         <v>19</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F38" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G38" s="7" t="s">
         <v>18</v>
@@ -2967,22 +2970,22 @@
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C39" s="24" t="s">
         <v>29</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F39" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G39" s="7" t="s">
         <v>18</v>
@@ -3032,22 +3035,22 @@
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C40" s="24" t="s">
-        <v>49</v>
-      </c>
       <c r="D40" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G40" s="7" t="s">
         <v>18</v>
@@ -3097,22 +3100,22 @@
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C41" s="24" t="s">
         <v>29</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F41" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G41" s="7" t="s">
         <v>18</v>
@@ -3121,7 +3124,7 @@
         <v>1</v>
       </c>
       <c r="I41" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J41" s="13">
         <f t="shared" si="18"/>
@@ -3162,22 +3165,22 @@
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E42" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>18</v>
@@ -3186,7 +3189,7 @@
         <v>1</v>
       </c>
       <c r="I42" s="34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J42" s="13">
         <f t="shared" si="18"/>
@@ -3230,19 +3233,19 @@
         <v>32</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C43" s="24" t="s">
         <v>19</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>18</v>
@@ -3342,16 +3345,16 @@
       <c r="J46" s="13"/>
       <c r="K46" s="3"/>
       <c r="L46" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M46" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="M46" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
       <c r="R46" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S46" s="1"/>
     </row>
@@ -3379,8 +3382,8 @@
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
       <c r="R47" s="20">
-        <f>SUM(R33:R42)</f>
-        <v>2740000.0199999996</v>
+        <f>SUM(R33:R43)</f>
+        <v>3839999.9999999995</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
@@ -3407,22 +3410,22 @@
         <v>33</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C49" s="24" t="s">
         <v>29</v>
       </c>
       <c r="D49" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E49" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E49" s="14" t="s">
-        <v>55</v>
-      </c>
       <c r="F49" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H49" s="28">
         <v>2</v>
@@ -3468,31 +3471,31 @@
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>34</v>
+        <v>118</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C50" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F50" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H50" s="29">
         <v>1</v>
       </c>
       <c r="I50" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J50" s="13">
         <f t="shared" si="27"/>
@@ -3504,7 +3507,7 @@
       </c>
       <c r="L50" s="2" t="str">
         <f t="shared" si="28"/>
-        <v xml:space="preserve">CHING CHONG    </v>
+        <v xml:space="preserve">DAVIS          </v>
       </c>
       <c r="M50" s="2" t="str">
         <f t="shared" si="29"/>
@@ -3533,7 +3536,7 @@
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>12</v>
@@ -3542,22 +3545,22 @@
         <v>19</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F51" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H51" s="29">
         <v>2</v>
       </c>
       <c r="I51" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J51" s="13">
         <f t="shared" si="27"/>
@@ -3598,25 +3601,25 @@
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C52" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E52" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F52" s="16" t="s">
         <v>22</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H52" s="29">
         <v>3</v>
@@ -3663,31 +3666,31 @@
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C53" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D53" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E53" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="E53" s="15" t="s">
+      <c r="F53" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="F53" s="16" t="s">
-        <v>108</v>
-      </c>
       <c r="G53" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H53" s="29">
         <v>1</v>
       </c>
       <c r="I53" s="34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J53" s="13">
         <f t="shared" si="27"/>
@@ -3728,7 +3731,7 @@
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>17</v>
@@ -3737,16 +3740,16 @@
         <v>19</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E54" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F54" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H54" s="29">
         <v>3</v>
@@ -3793,25 +3796,25 @@
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C55" s="24" t="s">
         <v>29</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E55" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F55" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H55" s="29">
         <v>3</v>
@@ -3858,25 +3861,25 @@
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B56" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C56" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C56" s="24" t="s">
-        <v>49</v>
-      </c>
       <c r="D56" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E56" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F56" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H56" s="29">
         <v>1</v>
@@ -3923,31 +3926,31 @@
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C57" s="24" t="s">
         <v>29</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E57" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F57" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H57" s="29">
         <v>1</v>
       </c>
       <c r="I57" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J57" s="13">
         <f t="shared" si="27"/>
@@ -3988,31 +3991,31 @@
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C58" s="24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E58" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F58" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="G58" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="G58" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="H58" s="29">
         <v>2</v>
       </c>
       <c r="I58" s="34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J58" s="13">
         <f t="shared" si="27"/>
@@ -4056,22 +4059,22 @@
         <v>32</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C59" s="24" t="s">
         <v>19</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E59" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F59" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H59" s="28">
         <v>1</v>
@@ -4168,16 +4171,16 @@
       <c r="J62" s="13"/>
       <c r="K62" s="3"/>
       <c r="L62" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M62" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="M62" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="O62" s="2"/>
       <c r="P62" s="2"/>
       <c r="Q62" s="2"/>
       <c r="R62" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
@@ -4204,8 +4207,8 @@
       <c r="P63" s="2"/>
       <c r="Q63" s="2"/>
       <c r="R63" s="20">
-        <f>SUM(R49:R58)</f>
-        <v>2292000.0199999996</v>
+        <f>SUM(R49:R59)</f>
+        <v>3391999.9999999995</v>
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
@@ -4236,22 +4239,22 @@
         <v>33</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C66" s="24" t="s">
         <v>29</v>
       </c>
       <c r="D66" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E66" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E66" s="14" t="s">
-        <v>55</v>
-      </c>
       <c r="F66" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H66" s="28">
         <v>2</v>
@@ -4297,31 +4300,31 @@
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>34</v>
+        <v>118</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C67" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E67" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F67" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H67" s="29">
         <v>1</v>
       </c>
       <c r="I67" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J67" s="13">
         <f t="shared" si="36"/>
@@ -4333,7 +4336,7 @@
       </c>
       <c r="L67" s="2" t="str">
         <f t="shared" si="37"/>
-        <v xml:space="preserve">CHING CHONG    </v>
+        <v xml:space="preserve">DAVIS          </v>
       </c>
       <c r="M67" s="2" t="str">
         <f t="shared" si="38"/>
@@ -4362,31 +4365,31 @@
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C68" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="B68" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C68" s="24" t="s">
+      <c r="D68" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="D68" s="9" t="s">
+      <c r="E68" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F68" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="E68" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="F68" s="16" t="s">
+      <c r="G68" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="H68" s="29">
         <v>3</v>
       </c>
       <c r="I68" s="34" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J68" s="13">
         <f t="shared" si="36"/>
@@ -4427,7 +4430,7 @@
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>12</v>
@@ -4436,22 +4439,22 @@
         <v>19</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E69" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F69" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H69" s="29">
         <v>2</v>
       </c>
       <c r="I69" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J69" s="13">
         <f t="shared" si="36"/>
@@ -4492,25 +4495,25 @@
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C70" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E70" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F70" s="16" t="s">
         <v>22</v>
       </c>
       <c r="G70" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H70" s="29">
         <v>3</v>
@@ -4557,7 +4560,7 @@
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>17</v>
@@ -4566,16 +4569,16 @@
         <v>19</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E71" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F71" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G71" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H71" s="29">
         <v>3</v>
@@ -4622,25 +4625,25 @@
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C72" s="24" t="s">
         <v>29</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E72" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F72" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G72" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H72" s="29">
         <v>3</v>
@@ -4687,25 +4690,25 @@
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B73" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C73" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C73" s="24" t="s">
-        <v>49</v>
-      </c>
       <c r="D73" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E73" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F73" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G73" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H73" s="29">
         <v>1</v>
@@ -4752,31 +4755,31 @@
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C74" s="24" t="s">
         <v>29</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E74" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F74" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G74" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H74" s="29">
         <v>1</v>
       </c>
       <c r="I74" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J74" s="13">
         <f t="shared" si="36"/>
@@ -4817,31 +4820,31 @@
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C75" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E75" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F75" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G75" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H75" s="29">
         <v>1</v>
       </c>
       <c r="I75" s="34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J75" s="13">
         <f t="shared" si="36"/>
@@ -4885,22 +4888,22 @@
         <v>32</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C76" s="24" t="s">
         <v>19</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E76" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F76" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H76" s="28">
         <v>1</v>
@@ -4977,16 +4980,16 @@
       <c r="J78" s="13"/>
       <c r="K78" s="3"/>
       <c r="L78" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M78" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="M78" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="O78" s="2"/>
       <c r="P78" s="2"/>
       <c r="Q78" s="2"/>
       <c r="R78" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S78" s="1"/>
     </row>
@@ -5007,15 +5010,15 @@
         <v>Cabin Cruiser</v>
       </c>
       <c r="M79" s="2">
-        <f>K75</f>
-        <v>10</v>
+        <f>K76</f>
+        <v>11</v>
       </c>
       <c r="O79" s="2"/>
       <c r="P79" s="2"/>
       <c r="Q79" s="2"/>
       <c r="R79" s="20">
-        <f>SUM(R65:R75)</f>
-        <v>2376000.0199999996</v>
+        <f>SUM(R65:R76)</f>
+        <v>3475999.9999999995</v>
       </c>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.25">
@@ -5047,27 +5050,27 @@
         <v>33</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C82" s="24" t="s">
         <v>29</v>
       </c>
       <c r="D82" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E82" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E82" s="14" t="s">
-        <v>55</v>
-      </c>
       <c r="F82" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H82" s="28">
         <v>2</v>
       </c>
-      <c r="I82" s="39" t="s">
+      <c r="I82" s="36" t="s">
         <v>30</v>
       </c>
       <c r="J82" s="13">
@@ -5108,31 +5111,31 @@
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>34</v>
+        <v>118</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C83" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D83" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E83" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F83" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H83" s="29">
         <v>1</v>
       </c>
       <c r="I83" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J83" s="13">
         <f t="shared" si="45"/>
@@ -5144,7 +5147,7 @@
       </c>
       <c r="L83" s="2" t="str">
         <f t="shared" si="46"/>
-        <v xml:space="preserve">CHING CHONG    </v>
+        <v xml:space="preserve">DAVIS          </v>
       </c>
       <c r="M83" s="2" t="str">
         <f t="shared" si="47"/>
@@ -5173,7 +5176,7 @@
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>12</v>
@@ -5182,22 +5185,22 @@
         <v>19</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E84" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F84" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G84" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H84" s="29">
         <v>2</v>
       </c>
       <c r="I84" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J84" s="13">
         <f t="shared" si="45"/>
@@ -5238,25 +5241,25 @@
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C85" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D85" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E85" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F85" s="16" t="s">
         <v>22</v>
       </c>
       <c r="G85" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H85" s="29">
         <v>3</v>
@@ -5303,31 +5306,31 @@
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B86" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C86" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="D86" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E86" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="D86" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="E86" s="15" t="s">
-        <v>117</v>
-      </c>
       <c r="F86" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G86" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H86" s="29">
         <v>3</v>
       </c>
       <c r="I86" s="34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J86" s="13">
         <f t="shared" si="45"/>
@@ -5368,7 +5371,7 @@
     </row>
     <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>17</v>
@@ -5377,16 +5380,16 @@
         <v>19</v>
       </c>
       <c r="D87" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E87" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F87" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G87" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H87" s="29">
         <v>3</v>
@@ -5433,25 +5436,25 @@
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C88" s="24" t="s">
         <v>29</v>
       </c>
       <c r="D88" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E88" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F88" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G88" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H88" s="29">
         <v>3</v>
@@ -5498,25 +5501,25 @@
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B89" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C89" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C89" s="24" t="s">
-        <v>49</v>
-      </c>
       <c r="D89" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E89" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F89" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G89" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H89" s="29">
         <v>1</v>
@@ -5563,31 +5566,31 @@
     </row>
     <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C90" s="24" t="s">
         <v>29</v>
       </c>
       <c r="D90" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E90" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F90" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G90" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H90" s="29">
         <v>1</v>
       </c>
       <c r="I90" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J90" s="13">
         <f t="shared" si="45"/>
@@ -5628,31 +5631,31 @@
     </row>
     <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C91" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D91" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E91" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E91" s="15" t="s">
+      <c r="F91" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="F91" s="15" t="s">
-        <v>56</v>
-      </c>
       <c r="G91" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H91" s="29">
         <v>3</v>
       </c>
       <c r="I91" s="34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J91" s="13">
         <f t="shared" si="45"/>
@@ -5696,22 +5699,22 @@
         <v>32</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C92" s="24" t="s">
         <v>19</v>
       </c>
       <c r="D92" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E92" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F92" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H92" s="28">
         <v>1</v>
@@ -5788,16 +5791,16 @@
       <c r="J94" s="13"/>
       <c r="K94" s="3"/>
       <c r="L94" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M94" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="M94" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="O94" s="2"/>
       <c r="P94" s="2"/>
       <c r="Q94" s="2"/>
       <c r="R94" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S94" s="1"/>
     </row>
@@ -5818,15 +5821,15 @@
         <v>Canoe</v>
       </c>
       <c r="M95" s="2">
-        <f>K91</f>
-        <v>10</v>
+        <f>K92</f>
+        <v>11</v>
       </c>
       <c r="O95" s="2"/>
       <c r="P95" s="2"/>
       <c r="Q95" s="2"/>
       <c r="R95" s="20">
-        <f>SUM(R81:R91)</f>
-        <v>2295250.0199999996</v>
+        <f>SUM(R81:R92)</f>
+        <v>3395249.9999999995</v>
       </c>
     </row>
     <row r="96" spans="1:19" x14ac:dyDescent="0.25">
@@ -5882,14 +5885,14 @@
       <c r="K98" s="3"/>
       <c r="L98" s="1"/>
       <c r="M98" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N98" s="2"/>
       <c r="O98" s="2"/>
       <c r="P98" s="2"/>
       <c r="Q98" s="2"/>
       <c r="R98" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.25">
@@ -5907,7 +5910,7 @@
       <c r="L99" s="1"/>
       <c r="M99" s="2">
         <f>M16+M31+M47+M63+M79+M95</f>
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="N99" s="2"/>
       <c r="O99" s="2"/>
@@ -5915,7 +5918,7 @@
       <c r="Q99" s="2"/>
       <c r="R99" s="20">
         <f>R16+R31+R47+R63+R79+R95</f>
-        <v>14351250.119999997</v>
+        <v>20951249.999999996</v>
       </c>
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>